<commit_message>
Hydroflask EMEA Test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/HydroflaskEMEA/HydroEMEATestData.xlsx
+++ b/src/test/resources/TestData/HydroflaskEMEA/HydroEMEATestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FE5B94-79CA-498A-80DB-73A7D1F4936D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2928E3A-A6B7-4281-899F-AC0D193127F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20580" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="142">
   <si>
     <t>UserName</t>
   </si>
@@ -320,9 +320,6 @@
     <t>MasterCard</t>
   </si>
   <si>
-    <t>5111005111051128</t>
-  </si>
-  <si>
     <t>Ccmastercard</t>
   </si>
   <si>
@@ -401,7 +398,61 @@
     <t>VisaCC</t>
   </si>
   <si>
-    <t>19Hyndu@98</t>
+    <t>narravivek168@gmail.com</t>
+  </si>
+  <si>
+    <t>Abcd1234</t>
+  </si>
+  <si>
+    <t>2222 4000 1000 0008</t>
+  </si>
+  <si>
+    <t>Searchmodel</t>
+  </si>
+  <si>
+    <t>Herr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 oz </t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>25 to 34</t>
+  </si>
+  <si>
+    <t>Über die Flasche</t>
+  </si>
+  <si>
+    <t>Technischer Support</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Utilisation de ma bouteille</t>
+  </si>
+  <si>
+    <t>J’ai une question technique</t>
+  </si>
+  <si>
+    <t>salutation_DE</t>
+  </si>
+  <si>
+    <t>salutation_FR</t>
+  </si>
+  <si>
+    <t>Type_FR</t>
+  </si>
+  <si>
+    <t>category_Demand_FR</t>
+  </si>
+  <si>
+    <t>Type_DE</t>
+  </si>
+  <si>
+    <t>category_Demand_DE</t>
   </si>
 </sst>
 </file>
@@ -411,7 +462,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,6 +481,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -462,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -482,6 +539,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -763,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AZ19"/>
+  <dimension ref="A1:BG20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="BF7" sqref="BF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,24 +861,29 @@
     <col min="31" max="31" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.7109375" customWidth="1"/>
-    <col min="37" max="37" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="21.140625" customWidth="1"/>
-    <col min="39" max="39" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="146.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="29.28515625" customWidth="1"/>
+    <col min="38" max="38" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.7109375" customWidth="1"/>
+    <col min="40" max="40" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.140625" customWidth="1"/>
+    <col min="42" max="42" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="146.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="18.85546875" customWidth="1"/>
+    <col min="57" max="57" width="14.7109375" customWidth="1"/>
+    <col min="58" max="58" width="26" customWidth="1"/>
+    <col min="59" max="59" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -897,7 +963,7 @@
         <v>18</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>19</v>
@@ -921,66 +987,87 @@
         <v>52</v>
       </c>
       <c r="AI1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AV1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AY1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="BC1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>124</v>
@@ -992,7 +1079,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1004,7 +1091,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -1046,7 +1133,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1088,16 +1175,19 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>117</v>
       </c>
       <c r="C5" s="1"/>
       <c r="W5" t="s">
         <v>96</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="Y5" s="3">
         <v>30</v>
@@ -1105,38 +1195,41 @@
       <c r="Z5" t="s">
         <v>24</v>
       </c>
+      <c r="AA5" s="6" t="s">
+        <v>120</v>
+      </c>
       <c r="AB5" s="4">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" s="1"/>
       <c r="W6" t="s">
         <v>22</v>
       </c>
       <c r="X6" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y6" s="6">
         <v>30</v>
       </c>
       <c r="Z6" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA6" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="AA6" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="AB6" s="4">
         <v>737</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:59" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1189,7 +1282,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1241,7 +1334,7 @@
         <v>9898989899</v>
       </c>
     </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1298,74 +1391,95 @@
       <c r="AH9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AI9" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>133</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>131</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>132</v>
+      </c>
+      <c r="BF9" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>61</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AL11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:52" s="8" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:59" s="8" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>72</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AJ12" s="8" t="s">
+      <c r="AM12" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="AK12" s="8" t="s">
+      <c r="AN12" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="AL12" s="9" t="s">
+      <c r="AO12" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="AM12" s="8" t="s">
+      <c r="AP12" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="AN12" s="8" t="s">
+      <c r="AQ12" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="AO12" s="8" t="s">
+      <c r="AR12" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="AP12" s="8">
-        <v>27</v>
-      </c>
-      <c r="AQ12" s="8" t="s">
+      <c r="AS12" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AT12" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="AR12" s="8" t="s">
+      <c r="AU12" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="AS12" s="8" t="s">
+      <c r="AV12" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="AT12" s="8">
+      <c r="AW12" s="8">
         <v>2</v>
       </c>
-      <c r="AU12" s="8" t="s">
+      <c r="AX12" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>86</v>
       </c>
@@ -1375,7 +1489,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1398,9 +1512,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
+      </c>
+      <c r="B15" t="s">
+        <v>117</v>
       </c>
       <c r="C15" s="1"/>
       <c r="W15" t="s">
@@ -1410,80 +1527,88 @@
         <v>93</v>
       </c>
       <c r="Y15" s="3">
-        <v>2025</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>24</v>
+        <v>123</v>
+      </c>
+      <c r="AA15" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="AB15" s="4">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV16" t="s">
+        <v>100</v>
+      </c>
+      <c r="AY16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>104</v>
-      </c>
-      <c r="AW17" t="s">
+      <c r="AZ17" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>109</v>
+      </c>
+      <c r="BB17" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AX17" t="s">
+    </row>
+    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
+      <c r="AZ18" t="s">
         <v>110</v>
       </c>
-      <c r="AY17" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="BA18" t="s">
+        <v>111</v>
+      </c>
+      <c r="BB18" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>114</v>
       </c>
-      <c r="AW18" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX18" t="s">
-        <v>112</v>
-      </c>
-      <c r="AY18" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>115</v>
-      </c>
-      <c r="AZ19" t="s">
-        <v>117</v>
+      <c r="BC19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>129</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="F4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="F7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C7" r:id="rId6" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C8" r:id="rId7" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="F8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="I8" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F3" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F13" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F14" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="G14" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="AY17" r:id="rId16" xr:uid="{F5CD1D5B-EDF7-4830-BA0B-5F7528F53E53}"/>
-    <hyperlink ref="AY18" r:id="rId17" xr:uid="{C1610D07-FC6B-451B-969C-F66269F656AB}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId4" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId5" display="Mahendra@123.com" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F3" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="BB17" r:id="rId14" xr:uid="{F5CD1D5B-EDF7-4830-BA0B-5F7528F53E53}"/>
+    <hyperlink ref="BB18" r:id="rId15" xr:uid="{C1610D07-FC6B-451B-969C-F66269F656AB}"/>
+    <hyperlink ref="F2" r:id="rId16" xr:uid="{938A0708-A8EF-4615-9A8C-40AACED59B3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>